<commit_message>
se agrega excel y una parte de los permisos
</commit_message>
<xml_diff>
--- a/Analisis/indicadores lluvia.xlsx
+++ b/Analisis/indicadores lluvia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A92899-5AAF-4EBC-A314-6817159B569A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758D90EE-2EEB-4535-9A02-564CEB2FDF0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{56216E52-3018-4F4A-897D-AA49E08DEF5D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{56216E52-3018-4F4A-897D-AA49E08DEF5D}"/>
   </bookViews>
   <sheets>
     <sheet name="compras" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
   <si>
     <t>fecha</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Proveedor</t>
   </si>
   <si>
-    <t>Tipo de ciente</t>
-  </si>
-  <si>
     <t>Nombre del cliente</t>
   </si>
   <si>
@@ -227,9 +224,6 @@
     <t>Persona que procesa la devolución</t>
   </si>
   <si>
-    <t>Precion / costo compra</t>
-  </si>
-  <si>
     <t>Tipo de cliente</t>
   </si>
   <si>
@@ -258,6 +252,24 @@
   </si>
   <si>
     <t>monto de compras =  ultimo costo de compra?</t>
+  </si>
+  <si>
+    <t>Precio / costo compra</t>
+  </si>
+  <si>
+    <t>Date Range</t>
+  </si>
+  <si>
+    <t>el ultimo precio compra</t>
+  </si>
+  <si>
+    <t>Es Utilidad ? Que pasa con los rangos de precios</t>
+  </si>
+  <si>
+    <t>como obtener el numero de clientes  ? Pòr que puede aparecer el mismo clientes en diferentes tickets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">como obtener ventas ya que existe un rango de precios y afecta directamente el precio con que se vende ese producto </t>
   </si>
 </sst>
 </file>
@@ -770,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A45CB0-F4D7-E44C-BA50-A59C65C29D74}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -785,10 +797,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -806,14 +818,14 @@
         <v>3</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -893,7 +905,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -906,13 +918,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
@@ -927,10 +939,10 @@
         <v>2</v>
       </c>
       <c r="I1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +955,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -961,19 +973,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>17</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>4</v>
@@ -993,7 +1005,7 @@
     </row>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
       <c r="C2" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
@@ -1010,7 +1022,7 @@
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1018,17 +1030,17 @@
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1036,7 +1048,7 @@
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1061,7 +1073,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:L7"/>
+      <selection activeCell="L3" sqref="B3:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1071,22 +1083,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -1101,7 +1113,7 @@
         <v>3</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1114,7 +1126,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G1" sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1141,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1141,29 +1153,29 @@
         <v>4</v>
       </c>
       <c r="F1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>55</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -1205,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B826896E-82E3-A247-A364-739C7C42C4FD}">
-  <dimension ref="B1:L46"/>
+  <dimension ref="B1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -1220,161 +1232,167 @@
     <col min="12" max="12" width="41.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.4">
       <c r="L1" s="20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.4">
       <c r="L2" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+      <c r="M4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
       <c r="L5" s="19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
+        <v>66</v>
+      </c>
+      <c r="M5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6">
         <v>360</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2">
         <v>1000</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="2">
         <v>1000</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2">
         <v>500</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8" s="2">
         <v>1200</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2">
         <v>250</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:13" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C11" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="7">
         <f>(D9*D6)/D8</f>
         <v>15</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11">
         <f>(H9*H6)/H8</f>
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:13" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C12" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="9">
         <f>30/D11</f>
         <v>2</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H12">
         <f>30/H11</f>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B15" s="5">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L15" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.4">
       <c r="C17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.4">
       <c r="C18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18">
         <v>1500</v>
@@ -1382,7 +1400,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.4">
       <c r="C19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19">
         <v>1000</v>
@@ -1390,7 +1408,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.4">
       <c r="C20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20">
         <f>D18-D19</f>
@@ -1399,7 +1417,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.4">
       <c r="C21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D21">
         <v>400</v>
@@ -1407,7 +1425,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.4">
       <c r="C22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22">
         <f>D20-D21</f>
@@ -1416,7 +1434,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.4">
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="2">
         <v>5</v>
@@ -1425,7 +1443,7 @@
     <row r="24" spans="2:4" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="25" spans="2:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C25" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="11">
         <f>(D22*D23)/(D18*D23)</f>
@@ -1437,17 +1455,17 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.4">
       <c r="C28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.4">
       <c r="C30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" s="2">
         <v>8</v>
@@ -1455,83 +1473,92 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.4">
       <c r="C32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="4">
         <f>D19*D30</f>
         <v>8000</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D33" s="4">
         <f>D19*D23</f>
         <v>5000</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="L33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" s="4">
         <f>D32-D33</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="36" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:12" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="36" spans="2:12" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C36" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D36" s="11">
         <f>D34/D32</f>
         <v>0.375</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="L36" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B38" s="5">
         <v>5</v>
       </c>
       <c r="C38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C40" t="s">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C42" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="C42" t="s">
-        <v>47</v>
       </c>
       <c r="D42">
         <v>1500</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="44" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="L42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="44" spans="2:12" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C44" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D44" s="13">
         <f>D32/D42</f>
         <v>5.333333333333333</v>
       </c>
       <c r="E44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="F45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="F45" t="s">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="F46" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="F46" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion de inventario promedio diario
</commit_message>
<xml_diff>
--- a/Analisis/indicadores lluvia.xlsx
+++ b/Analisis/indicadores lluvia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E523ABF9-7502-4E0E-8A6A-0253FE7A434D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8EC704-8A6F-4EBF-867A-D70331CE44ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="945" windowWidth="13305" windowHeight="11175" firstSheet="2" activeTab="5" xr2:uid="{56216E52-3018-4F4A-897D-AA49E08DEF5D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="3" activeTab="5" xr2:uid="{56216E52-3018-4F4A-897D-AA49E08DEF5D}"/>
   </bookViews>
   <sheets>
     <sheet name="compras" sheetId="1" r:id="rId1"/>
@@ -534,13 +534,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -982,7 +982,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J14"/>
+      <selection activeCell="A2" sqref="A2:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1150,7 +1150,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L13"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1296,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B826896E-82E3-A247-A364-739C7C42C4FD}">
   <dimension ref="B1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -1613,10 +1613,10 @@
       <c r="E32">
         <v>30</v>
       </c>
-      <c r="F32" s="23" t="s">
+      <c r="F32" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="G32" s="23"/>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C33" t="s">
@@ -1655,7 +1655,7 @@
         <f>D34/D32</f>
         <v>0.375</v>
       </c>
-      <c r="E36" s="24">
+      <c r="E36" s="22">
         <f>E34/E32</f>
         <v>0.46666666666666667</v>
       </c>
@@ -1670,13 +1670,13 @@
       <c r="C38" t="s">
         <v>44</v>
       </c>
-      <c r="I38" s="22" t="s">
+      <c r="I38" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.4">
       <c r="J39" t="s">

</xml_diff>

<commit_message>
se ajustan los calculos del  inventario promedio
</commit_message>
<xml_diff>
--- a/Analisis/indicadores lluvia.xlsx
+++ b/Analisis/indicadores lluvia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8EC704-8A6F-4EBF-867A-D70331CE44ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B8C1F6-93B8-496A-90BA-47321BF4A19B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="3" activeTab="5" xr2:uid="{56216E52-3018-4F4A-897D-AA49E08DEF5D}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="15750" firstSheet="3" activeTab="5" xr2:uid="{56216E52-3018-4F4A-897D-AA49E08DEF5D}"/>
   </bookViews>
   <sheets>
     <sheet name="compras" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>ejemplo para mes:</t>
   </si>
   <si>
-    <t xml:space="preserve">Dias promedio de inventario: (costo del inventario promedio * dias del periodo)/costo de ventas </t>
-  </si>
-  <si>
     <t>Rotación de inventarios: dias del periodo / dias promedio de inventario</t>
   </si>
   <si>
@@ -333,6 +330,9 @@
   </si>
   <si>
     <t>Producto = Agrupado ennuevo reporte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dias promedio de inventario: (costo del inventario promedio * dias del periodo)/costo de lo vendido </t>
   </si>
 </sst>
 </file>
@@ -874,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>15</v>
@@ -895,7 +895,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45.75" x14ac:dyDescent="0.25">
@@ -995,13 +995,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
@@ -1016,10 +1016,10 @@
         <v>2</v>
       </c>
       <c r="I1" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1056,13 +1056,13 @@
         <v>17</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>4</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
@@ -1163,19 +1163,19 @@
         <v>14</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -1190,7 +1190,7 @@
         <v>3</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1230,10 +1230,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1296,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B826896E-82E3-A247-A364-739C7C42C4FD}">
   <dimension ref="B1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -1313,12 +1313,12 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.4">
       <c r="L1" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.4">
       <c r="L2" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.4">
@@ -1326,13 +1326,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.4">
@@ -1340,21 +1340,21 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.4">
       <c r="L5" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.4">
@@ -1365,16 +1365,16 @@
         <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6">
         <v>360</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L6" s="19"/>
     </row>
@@ -1392,7 +1392,7 @@
         <v>1000</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.4">
@@ -1426,14 +1426,14 @@
     <row r="10" spans="2:13" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="11" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C11" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="7">
         <f>(D9*D6)/D8</f>
         <v>15</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11">
         <f>(H9*H6)/H8</f>
@@ -1461,23 +1461,23 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L15" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18">
         <v>1500</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <v>1000</v>
@@ -1494,30 +1494,30 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" t="s">
+        <v>79</v>
+      </c>
+      <c r="K19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" t="s">
+        <v>81</v>
+      </c>
+      <c r="M19" t="s">
+        <v>32</v>
+      </c>
+      <c r="N19" t="s">
         <v>83</v>
       </c>
-      <c r="J19" t="s">
-        <v>80</v>
-      </c>
-      <c r="K19" t="s">
-        <v>81</v>
-      </c>
-      <c r="L19" t="s">
-        <v>82</v>
-      </c>
-      <c r="M19" t="s">
-        <v>33</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>84</v>
-      </c>
-      <c r="O19" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20">
         <f>D18-D19</f>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21">
         <v>400</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22">
         <f>D20-D21</f>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="2">
         <v>5</v>
@@ -1552,7 +1552,7 @@
     <row r="24" spans="2:15" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="25" spans="2:15" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C25" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="11">
         <f>(D22*D23)/(D18*D23)</f>
@@ -1564,47 +1564,47 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.4">
       <c r="G29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" s="2">
         <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.4">
       <c r="G31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="4">
         <f>D19*D30</f>
@@ -1614,13 +1614,13 @@
         <v>30</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G32" s="24"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" s="4">
         <f>D19*D23</f>
@@ -1630,12 +1630,12 @@
         <v>16</v>
       </c>
       <c r="L33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D34" s="4">
         <f>D32-D33</f>
@@ -1649,7 +1649,7 @@
     <row r="35" spans="2:14" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="36" spans="2:14" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C36" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="11">
         <f>D34/D32</f>
@@ -1660,7 +1660,7 @@
         <v>0.46666666666666667</v>
       </c>
       <c r="L36" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.4">
@@ -1668,10 +1668,10 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I38" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J38" s="23"/>
       <c r="K38" s="23"/>
@@ -1680,58 +1680,58 @@
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.4">
       <c r="J39" t="s">
+        <v>89</v>
+      </c>
+      <c r="K39" t="s">
         <v>90</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>91</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>92</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>93</v>
-      </c>
-      <c r="N39" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D42">
         <v>1500</v>
       </c>
       <c r="L42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="2:14" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="44" spans="2:14" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C44" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D44" s="13">
         <f>D32/D42</f>
         <v>5.333333333333333</v>
       </c>
       <c r="E44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.4">
       <c r="F45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.4">
       <c r="F46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se hace commit derivado del merge
</commit_message>
<xml_diff>
--- a/Analisis/indicadores lluvia.xlsx
+++ b/Analisis/indicadores lluvia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E523ABF9-7502-4E0E-8A6A-0253FE7A434D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B8C1F6-93B8-496A-90BA-47321BF4A19B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="945" windowWidth="13305" windowHeight="11175" firstSheet="2" activeTab="5" xr2:uid="{56216E52-3018-4F4A-897D-AA49E08DEF5D}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="15750" firstSheet="3" activeTab="5" xr2:uid="{56216E52-3018-4F4A-897D-AA49E08DEF5D}"/>
   </bookViews>
   <sheets>
     <sheet name="compras" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>ejemplo para mes:</t>
   </si>
   <si>
-    <t xml:space="preserve">Dias promedio de inventario: (costo del inventario promedio * dias del periodo)/costo de ventas </t>
-  </si>
-  <si>
     <t>Rotación de inventarios: dias del periodo / dias promedio de inventario</t>
   </si>
   <si>
@@ -333,6 +330,9 @@
   </si>
   <si>
     <t>Producto = Agrupado ennuevo reporte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dias promedio de inventario: (costo del inventario promedio * dias del periodo)/costo de lo vendido </t>
   </si>
 </sst>
 </file>
@@ -534,13 +534,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -874,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>15</v>
@@ -895,7 +895,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45.75" x14ac:dyDescent="0.25">
@@ -982,7 +982,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J14"/>
+      <selection activeCell="A2" sqref="A2:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -995,13 +995,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
@@ -1016,10 +1016,10 @@
         <v>2</v>
       </c>
       <c r="I1" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1056,13 +1056,13 @@
         <v>17</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>4</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
@@ -1150,7 +1150,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L13"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1163,19 +1163,19 @@
         <v>14</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -1190,7 +1190,7 @@
         <v>3</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1230,10 +1230,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1296,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B826896E-82E3-A247-A364-739C7C42C4FD}">
   <dimension ref="B1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -1313,12 +1313,12 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.4">
       <c r="L1" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.4">
       <c r="L2" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.4">
@@ -1326,13 +1326,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.4">
@@ -1340,21 +1340,21 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.4">
       <c r="L5" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.4">
@@ -1365,16 +1365,16 @@
         <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6">
         <v>360</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L6" s="19"/>
     </row>
@@ -1392,7 +1392,7 @@
         <v>1000</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.4">
@@ -1426,14 +1426,14 @@
     <row r="10" spans="2:13" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="11" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C11" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="7">
         <f>(D9*D6)/D8</f>
         <v>15</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11">
         <f>(H9*H6)/H8</f>
@@ -1461,23 +1461,23 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L15" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18">
         <v>1500</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <v>1000</v>
@@ -1494,30 +1494,30 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" t="s">
+        <v>79</v>
+      </c>
+      <c r="K19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" t="s">
+        <v>81</v>
+      </c>
+      <c r="M19" t="s">
+        <v>32</v>
+      </c>
+      <c r="N19" t="s">
         <v>83</v>
       </c>
-      <c r="J19" t="s">
-        <v>80</v>
-      </c>
-      <c r="K19" t="s">
-        <v>81</v>
-      </c>
-      <c r="L19" t="s">
-        <v>82</v>
-      </c>
-      <c r="M19" t="s">
-        <v>33</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>84</v>
-      </c>
-      <c r="O19" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20">
         <f>D18-D19</f>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21">
         <v>400</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22">
         <f>D20-D21</f>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="2">
         <v>5</v>
@@ -1552,7 +1552,7 @@
     <row r="24" spans="2:15" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="25" spans="2:15" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C25" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="11">
         <f>(D22*D23)/(D18*D23)</f>
@@ -1564,47 +1564,47 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.4">
       <c r="G29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" s="2">
         <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.4">
       <c r="G31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="4">
         <f>D19*D30</f>
@@ -1613,14 +1613,14 @@
       <c r="E32">
         <v>30</v>
       </c>
-      <c r="F32" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="G32" s="23"/>
+      <c r="F32" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" s="4">
         <f>D19*D23</f>
@@ -1630,12 +1630,12 @@
         <v>16</v>
       </c>
       <c r="L33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D34" s="4">
         <f>D32-D33</f>
@@ -1649,18 +1649,18 @@
     <row r="35" spans="2:14" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="36" spans="2:14" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C36" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="11">
         <f>D34/D32</f>
         <v>0.375</v>
       </c>
-      <c r="E36" s="24">
+      <c r="E36" s="22">
         <f>E34/E32</f>
         <v>0.46666666666666667</v>
       </c>
       <c r="L36" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.4">
@@ -1668,70 +1668,70 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
-      </c>
-      <c r="I38" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
+        <v>43</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.4">
       <c r="J39" t="s">
+        <v>89</v>
+      </c>
+      <c r="K39" t="s">
         <v>90</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>91</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>92</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>93</v>
-      </c>
-      <c r="N39" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D42">
         <v>1500</v>
       </c>
       <c r="L42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="2:14" ht="27" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="44" spans="2:14" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C44" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D44" s="13">
         <f>D32/D42</f>
         <v>5.333333333333333</v>
       </c>
       <c r="E44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.4">
       <c r="F45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.4">
       <c r="F46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>